<commit_message>
Jags tables to 3 digits
</commit_message>
<xml_diff>
--- a/data/output_data/Invert_jags_summary_tables.xlsx
+++ b/data/output_data/Invert_jags_summary_tables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\maedward\Desktop\thesis\data\output_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maedward\Desktop\thesis\data\output_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21510" windowHeight="8985" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21516" windowHeight="8988" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CIPA_jags_summary_tables" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -672,7 +675,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -710,6 +713,19 @@
     <xf numFmtId="49" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1042,19 +1058,19 @@
       <selection pane="bottomLeft" activeCell="A17" sqref="A17:F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="4" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="4"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="9.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="4" customWidth="1"/>
+    <col min="7" max="9" width="9.109375" style="4"/>
+    <col min="10" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -1062,7 +1078,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1100,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1109,7 +1125,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1134,7 +1150,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1159,7 +1175,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1184,7 +1200,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1209,7 +1225,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1234,7 +1250,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1259,7 +1275,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1284,7 +1300,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1309,7 +1325,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1334,12 +1350,12 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -1364,7 +1380,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1372,7 +1388,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
         <v>19</v>
@@ -1390,7 +1406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>21</v>
       </c>
@@ -1400,7 +1416,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
@@ -1420,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>17</v>
       </c>
@@ -1440,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>18</v>
       </c>
@@ -1460,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1468,7 +1484,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>20</v>
       </c>
@@ -1478,7 +1494,7 @@
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>15</v>
       </c>
@@ -1498,7 +1514,7 @@
         <v>1.2193993473868401</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>17</v>
       </c>
@@ -1518,7 +1534,7 @@
         <v>1.0003524175421299</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>18</v>
       </c>
@@ -1538,7 +1554,7 @@
         <v>1.0009645219399499</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>22</v>
       </c>
@@ -1558,7 +1574,7 @@
         <v>1.0855776532943999</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1566,7 +1582,7 @@
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>23</v>
       </c>
@@ -1576,7 +1592,7 @@
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>24</v>
       </c>
@@ -1596,7 +1612,7 @@
         <v>1.0036039134971999</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>25</v>
       </c>
@@ -1616,7 +1632,7 @@
         <v>1.2822223437273099</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>26</v>
       </c>
@@ -1636,7 +1652,7 @@
         <v>1.32427694555789</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -1644,7 +1660,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -1667,16 +1683,16 @@
       <selection pane="bottomLeft" activeCell="A14" sqref="A14:F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1693,7 +1709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1713,7 +1729,7 @@
         <v>1.4225942048026099</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1733,7 +1749,7 @@
         <v>1.0416069197123801</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1753,7 +1769,7 @@
         <v>1.1587380920477199</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1773,7 +1789,7 @@
         <v>1.0531959147352801</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1793,7 +1809,7 @@
         <v>1.03198962847704</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1813,7 +1829,7 @@
         <v>1.0165872521397299</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1833,7 +1849,7 @@
         <v>1.0136099596153001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1853,7 +1869,7 @@
         <v>1.33348021396743</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1873,7 +1889,7 @@
         <v>1.08014744081531</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1893,7 +1909,7 @@
         <v>1.00203542995002</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="13" t="s">
         <v>19</v>
@@ -1911,7 +1927,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
@@ -1921,7 +1937,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>15</v>
       </c>
@@ -1941,7 +1957,7 @@
         <v>1.03198962847704</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>30</v>
       </c>
@@ -1961,7 +1977,7 @@
         <v>1.0165872521397299</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1969,7 +1985,7 @@
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>20</v>
       </c>
@@ -1979,7 +1995,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
@@ -1999,7 +2015,7 @@
         <v>1.4225942048026099</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>31</v>
       </c>
@@ -2019,7 +2035,7 @@
         <v>1.0416069197123801</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>30</v>
       </c>
@@ -2039,7 +2055,7 @@
         <v>1.0531959147352801</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>22</v>
       </c>
@@ -2059,7 +2075,7 @@
         <v>1.1587380920477199</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -2067,7 +2083,7 @@
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>23</v>
       </c>
@@ -2077,7 +2093,7 @@
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>24</v>
       </c>
@@ -2097,7 +2113,7 @@
         <v>1.0136099596153001</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
@@ -2117,7 +2133,7 @@
         <v>1.33348021396743</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>26</v>
       </c>
@@ -2147,20 +2163,20 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="A20" sqref="A20:F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="20" t="s">
         <v>19</v>
@@ -2178,7 +2194,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -2188,460 +2204,480 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="21">
         <v>-0.12346970491685599</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="21">
         <v>0.31335925737020598</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="21">
         <v>-0.73618925497998</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="21">
         <v>0.49425494696593503</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="22">
         <v>0.67060431777477003</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="22">
         <v>0.323484753635009</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="22">
         <v>5.9855812873922297E-2</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="22">
         <v>1.33616637254355</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="22">
         <v>0.75261930143250999</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="22">
         <v>0.33980087222677702</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="22">
         <v>0.119669998776116</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="22">
         <v>1.4559106180203001</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="21">
         <v>13.2375336350292</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="21">
         <v>11.172271584154601</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="21">
         <v>1.729641467854</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="21">
         <v>42.447351384178198</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="21">
         <v>1.2193993473868401</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="22">
         <v>0.67060431777477003</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="22">
         <v>0.323484753635009</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="22">
         <v>5.9855812873922297E-2</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="22">
         <v>1.33616637254355</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="22">
         <v>1.0003524175421299</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="22">
         <v>0.75261930143250999</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="22">
         <v>0.33980087222677702</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="22">
         <v>0.119669998776116</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="22">
         <v>1.4559106180203001</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="22">
         <v>1.0009645219399499</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="22">
         <v>2.04047858110872</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="22">
         <v>0.290637878672383</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="22">
         <v>1.5555880904152599</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="22">
         <v>2.7316400844021298</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="22">
         <v>1.0855776532943999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="21">
         <v>0.57070406351719905</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="21">
         <v>0.11274490204665299</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="21">
         <v>0.37909528862079001</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="21">
         <v>0.81821627605843095</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="21">
         <v>1.0036039134971999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="22">
         <v>50.818958970454197</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="22">
         <v>40.261502610478701</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="22">
         <v>8.88424482119534</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="22">
         <v>179.90961466530601</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="22">
         <v>1.2822223437273099</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="24">
         <v>1.74494426034691E-2</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="24">
         <v>1.21110220582015E-2</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="24">
         <v>3.0855660527294099E-3</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="24">
         <v>4.9548122693676401E-2</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="24">
         <v>1.32427694555789</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="23">
         <v>0.97499999999999998</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="21">
         <v>-0.68710395030101701</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="21">
         <v>0.84213543474107999</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="21">
         <v>-2.0831685944235598</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="21">
         <v>1.21921205370501</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="21">
         <v>1.03198962847704</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="22">
         <v>2.50211498455884</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="22">
         <v>1.5543120464718501</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="22">
         <v>-0.26674071374422598</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="22">
         <v>5.7816779774986697</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="22">
         <v>1.0165872521397299</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="21">
         <v>11.113689642371501</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="21">
         <v>24.601518527389899</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="21">
         <v>2.4531058522491898E-2</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="21">
         <v>103.897965347425</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="21">
         <v>1.4225942048026099</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="22">
         <v>-3.7888889552299099</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="22">
         <v>1.2729541797655901</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="22">
         <v>-6.4927826835646298</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="22">
         <v>-1.4025711749323999</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="22">
         <v>1.0416069197123801</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="22">
         <v>0.91680581085428803</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="22">
         <v>0.763891494606876</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="22">
         <v>-0.37130255306016602</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="22">
         <v>2.5458624255578699</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="22">
         <v>1.0531959147352801</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="22">
         <v>1.61080006000733</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="22">
         <v>0.87946406928031295</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="22">
         <v>0.31083467107283402</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="22">
         <v>4.0206418532430703</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="22">
         <v>1.1587380920477199</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="16">
+      <c r="B30" s="21">
         <v>1.0420092645601899</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="21">
         <v>0.82159209354500995</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="21">
         <v>0.20490017700726901</v>
       </c>
-      <c r="E30" s="16">
+      <c r="E30" s="21">
         <v>3.2940744602952798</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F30" s="21">
         <v>1.0136099596153001</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="22">
         <v>52.309307347792902</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="22">
         <v>61.841148096238499</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="22">
         <v>3.9597541074559799</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="22">
         <v>248.74314975519999</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="22">
         <v>1.33348021396743</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="18">
+      <c r="B32" s="24">
         <v>3.31671443534882E-2</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="24">
         <v>2.30061998450127E-2</v>
       </c>
-      <c r="D32" s="18">
+      <c r="D32" s="24">
         <v>3.13175773539E-3</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="24">
         <v>9.2127661572020597E-2</v>
       </c>
-      <c r="F32" s="18">
+      <c r="F32" s="24">
         <v>1.08014744081531</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>